<commit_message>
Alle Teile da! :)
</commit_message>
<xml_diff>
--- a/Dokumentation/Schritte.xlsx
+++ b/Dokumentation/Schritte.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Datum</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>Blumen gebastelt. Wer braucht schon die Natur. Ab zum Datenerstellen</t>
+  </si>
+  <si>
+    <t>Alles Da.jpg; Angekommen.jpeg</t>
+  </si>
+  <si>
+    <t>Die Teile sind alle Da! Viel früher als erwartet. Auf die Chinesen ist verlass! Auf zum Löten (Raspi + Kamera fehlen)</t>
   </si>
 </sst>
 </file>
@@ -376,16 +382,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
     <col min="3" max="3" width="156.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -455,6 +461,17 @@
         <v>12</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>43058</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Platinen, Widerstände, Level Shifter
</commit_message>
<xml_diff>
--- a/Dokumentation/Schritte.xlsx
+++ b/Dokumentation/Schritte.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Datum</t>
   </si>
@@ -82,6 +82,24 @@
   </si>
   <si>
     <t>Hardware… Der Frust beginnt</t>
+  </si>
+  <si>
+    <t>Da ist noch etwas zu verbsessern :/</t>
+  </si>
+  <si>
+    <t>Blumigenachbarschaft.jpg</t>
+  </si>
+  <si>
+    <t>Geogebra_kontrast.jpg</t>
+  </si>
+  <si>
+    <t>Verschiedene auswahl für grauheitsberechnung der Pixel</t>
+  </si>
+  <si>
+    <t>Blume wird erkannt.jpg</t>
+  </si>
+  <si>
+    <t>Blume wird unter Optimalbedingungen erkannt. Müsste mit optimierungen und zusammenarbeit mit sensoren besser laufen</t>
   </si>
 </sst>
 </file>
@@ -400,20 +418,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
-    <col min="3" max="3" width="156.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="156.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,7 +442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43032</v>
       </c>
@@ -435,7 +453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43036</v>
       </c>
@@ -446,7 +464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43042</v>
       </c>
@@ -457,7 +475,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43017</v>
       </c>
@@ -468,7 +486,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43051</v>
       </c>
@@ -479,7 +497,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43058</v>
       </c>
@@ -490,7 +508,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43063</v>
       </c>
@@ -501,7 +519,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43063</v>
       </c>
@@ -512,7 +530,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43063</v>
       </c>
@@ -521,6 +539,39 @@
       </c>
       <c r="C10" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>43071</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>43071</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>43071</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I2C Addressen auf Kontrollschaltung
</commit_message>
<xml_diff>
--- a/Dokumentation/Schritte.xlsx
+++ b/Dokumentation/Schritte.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>Datum</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>Kontrollschaltung überarbeitet, gleicht nun gebautem</t>
+  </si>
+  <si>
+    <t>Addressen hinzugefügt</t>
   </si>
 </sst>
 </file>
@@ -484,20 +487,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
-    <col min="3" max="3" width="156.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="156.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -508,7 +511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43032</v>
       </c>
@@ -519,7 +522,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43036</v>
       </c>
@@ -530,7 +533,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43042</v>
       </c>
@@ -541,7 +544,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43017</v>
       </c>
@@ -552,7 +555,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43051</v>
       </c>
@@ -563,7 +566,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43058</v>
       </c>
@@ -574,7 +577,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43063</v>
       </c>
@@ -585,7 +588,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43063</v>
       </c>
@@ -596,7 +599,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43063</v>
       </c>
@@ -607,7 +610,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43071</v>
       </c>
@@ -618,7 +621,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43071</v>
       </c>
@@ -629,7 +632,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43071</v>
       </c>
@@ -640,7 +643,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43077</v>
       </c>
@@ -651,7 +654,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43078</v>
       </c>
@@ -662,7 +665,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43079</v>
       </c>
@@ -673,7 +676,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43090</v>
       </c>
@@ -684,7 +687,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43090</v>
       </c>
@@ -695,7 +698,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43090</v>
       </c>
@@ -706,7 +709,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43091</v>
       </c>
@@ -717,7 +720,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43091</v>
       </c>
@@ -728,7 +731,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43097</v>
       </c>
@@ -739,7 +742,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43097</v>
       </c>
@@ -750,7 +753,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43097</v>
       </c>
@@ -759,6 +762,17 @@
       </c>
       <c r="C24" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>42737</v>
+      </c>
+      <c r="B25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Einheitliche Namengebung in Dokumentation
</commit_message>
<xml_diff>
--- a/Dokumentation/Schritte.xlsx
+++ b/Dokumentation/Schritte.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="78">
   <si>
     <t>Datum</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Blumen gebastelt. Wer braucht schon die Natur. Ab zum Datenerstellen</t>
   </si>
   <si>
-    <t>Alles Da.jpg; Angekommen.jpeg</t>
-  </si>
-  <si>
     <t>Die Teile sind alle Da! Viel früher als erwartet. Auf die Chinesen ist verlass! Auf zum Löten (Raspi + Kamera fehlen)</t>
   </si>
   <si>
@@ -241,6 +238,21 @@
   </si>
   <si>
     <t>Optimierungen an C#-Programm durchgeführt</t>
+  </si>
+  <si>
+    <t>Angekommen.jpeg</t>
+  </si>
+  <si>
+    <t>Alles Da.jpg;</t>
+  </si>
+  <si>
+    <t>Die Excel Tabelle</t>
+  </si>
+  <si>
+    <t>2017-12.11.jpg</t>
+  </si>
+  <si>
+    <t>Raspberry Pi gehäuse fertig. Testdruck geschaftt. Etwas verspätet!</t>
   </si>
 </sst>
 </file>
@@ -559,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,7 +630,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>43017</v>
+        <v>43048</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -643,21 +655,21 @@
         <v>43058</v>
       </c>
       <c r="B7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" t="s">
         <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>43063</v>
+        <v>43058</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -665,10 +677,10 @@
         <v>43063</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -676,21 +688,21 @@
         <v>43063</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>43071</v>
+        <v>43063</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -698,10 +710,10 @@
         <v>43071</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -709,65 +721,65 @@
         <v>43071</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>43077</v>
+        <v>43071</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>43078</v>
+        <v>43077</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>43079</v>
+        <v>43078</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>43090</v>
+        <v>43079</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>43090</v>
+        <v>43080</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -775,54 +787,54 @@
         <v>43090</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>43091</v>
+        <v>43090</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>43091</v>
+        <v>43090</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>43097</v>
+        <v>43091</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>43097</v>
+        <v>43091</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -830,54 +842,54 @@
         <v>43097</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>43102</v>
+        <v>43097</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>43101</v>
+        <v>43097</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>43103</v>
+        <v>43102</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>43103</v>
+        <v>43101</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -885,10 +897,10 @@
         <v>43103</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -896,10 +908,10 @@
         <v>43103</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -907,10 +919,10 @@
         <v>43103</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -918,10 +930,10 @@
         <v>43103</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C32" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -929,54 +941,76 @@
         <v>43103</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>43104</v>
+        <v>43103</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C34" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>43105</v>
+        <v>43103</v>
       </c>
       <c r="B35" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>43107</v>
+        <v>43104</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C36" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
+        <v>43105</v>
+      </c>
+      <c r="B37" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
         <v>43107</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>43107</v>
+      </c>
+      <c r="B39" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" t="s">
         <v>72</v>
-      </c>
-      <c r="C37" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Antenne erprobt + funktionstüchtig
</commit_message>
<xml_diff>
--- a/Dokumentation/Schritte.xlsx
+++ b/Dokumentation/Schritte.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="156">
   <si>
     <t>Datum</t>
   </si>
@@ -462,6 +462,36 @@
   </si>
   <si>
     <t>Basisstation weiterentwickelt, probleme mit Arduino -&gt; Raspberry pi dazwischen</t>
+  </si>
+  <si>
+    <t>2018-04-21 1.PNG</t>
+  </si>
+  <si>
+    <t>Versuche über Senden und empfangen über RF</t>
+  </si>
+  <si>
+    <t>2018-04-21 2.PNG</t>
+  </si>
+  <si>
+    <t>ERFOLG! Die zahlen 0-32 werden erfolgreich übertragen</t>
+  </si>
+  <si>
+    <t>2018-04-21 3.JPG</t>
+  </si>
+  <si>
+    <t>Testsetup im Garten</t>
+  </si>
+  <si>
+    <t>2018-04-21 4.JPG</t>
+  </si>
+  <si>
+    <t>Testsetup im Garten andere Perspektive</t>
+  </si>
+  <si>
+    <t>2018-04-21 5.JPG</t>
+  </si>
+  <si>
+    <t>Übertragung über Antennen. Reichweite problematisch</t>
   </si>
 </sst>
 </file>
@@ -780,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1619,6 +1649,61 @@
         <v>145</v>
       </c>
     </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
+        <v>43211</v>
+      </c>
+      <c r="B76" t="s">
+        <v>146</v>
+      </c>
+      <c r="C76" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="1">
+        <v>43211</v>
+      </c>
+      <c r="B77" t="s">
+        <v>148</v>
+      </c>
+      <c r="C77" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="1">
+        <v>43211</v>
+      </c>
+      <c r="B78" t="s">
+        <v>150</v>
+      </c>
+      <c r="C78" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="1">
+        <v>43211</v>
+      </c>
+      <c r="B79" t="s">
+        <v>152</v>
+      </c>
+      <c r="C79" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="1">
+        <v>43211</v>
+      </c>
+      <c r="B80" t="s">
+        <v>154</v>
+      </c>
+      <c r="C80" t="s">
+        <v>155</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Datenübertragung Basis(PC) > Drohne(PI)
</commit_message>
<xml_diff>
--- a/Dokumentation/Schritte.xlsx
+++ b/Dokumentation/Schritte.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="169">
   <si>
     <t>Datum</t>
   </si>
@@ -525,6 +525,12 @@
   </si>
   <si>
     <t>Wir haben es in die Zeitung geschafft!</t>
+  </si>
+  <si>
+    <t>2018-04-28.PNG</t>
+  </si>
+  <si>
+    <t>Nach 7-8h rumprobieren, ENDLICH kommunikation zwischen PC und Drohne (Raspberry) muss ja noch zum nächsten Arduino</t>
   </si>
 </sst>
 </file>
@@ -843,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C86"/>
+  <dimension ref="A1:C87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1803,6 +1809,17 @@
         <v>166</v>
       </c>
     </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="1">
+        <v>43218</v>
+      </c>
+      <c r="B87" t="s">
+        <v>167</v>
+      </c>
+      <c r="C87" t="s">
+        <v>168</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Zweiseitige Kommunikation fertig. Rahmen gebaut
</commit_message>
<xml_diff>
--- a/Dokumentation/Schritte.xlsx
+++ b/Dokumentation/Schritte.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="173">
   <si>
     <t>Datum</t>
   </si>
@@ -531,6 +531,18 @@
   </si>
   <si>
     <t>Nach 7-8h rumprobieren, ENDLICH kommunikation zwischen PC und Drohne (Raspberry) muss ja noch zum nächsten Arduino</t>
+  </si>
+  <si>
+    <t>Ein Massiver und ein Leichter Ramen. Das Testen kann beginnen!</t>
+  </si>
+  <si>
+    <t>2018-04-29 1.JPG</t>
+  </si>
+  <si>
+    <t>2018-04-29 2.AVI</t>
+  </si>
+  <si>
+    <t>Die Kommunikation hin und zurück läuft! Drücken auf Start -&gt; Biep</t>
   </si>
 </sst>
 </file>
@@ -849,10 +861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C87"/>
+  <dimension ref="A1:C89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+      <selection activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1820,6 +1832,28 @@
         <v>168</v>
       </c>
     </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="1">
+        <v>43219</v>
+      </c>
+      <c r="B88" t="s">
+        <v>170</v>
+      </c>
+      <c r="C88" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="1">
+        <v>43219</v>
+      </c>
+      <c r="B89" t="s">
+        <v>171</v>
+      </c>
+      <c r="C89" t="s">
+        <v>172</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Kommunikation, Strommessung, Höhenmessung, YMFC Update
</commit_message>
<xml_diff>
--- a/Dokumentation/Schritte.xlsx
+++ b/Dokumentation/Schritte.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="195">
   <si>
     <t>Datum</t>
   </si>
@@ -591,6 +591,24 @@
   </si>
   <si>
     <t>Die Kommunikation von der Basis zum Arduino der Drohne (letztes programmiertes Glied der Kette vor der Hardware) funktioniert</t>
+  </si>
+  <si>
+    <t>Debuggen von diesen Großen konstrukten mit allen einzelteilen. Nur keine Panik!</t>
+  </si>
+  <si>
+    <t>2018-05-01 8.jpg</t>
+  </si>
+  <si>
+    <t>2018-05-01 9.jpg</t>
+  </si>
+  <si>
+    <t>Wenn mich die Hardware verlässt, kann die Zeit wenigstens für die Software verwendet werden. Es gibt jetzt eine stabile, relativ schnelle und zuverlässige zwei-Wege Kommunikation zwischen Basis und Arduino (Drohne)</t>
+  </si>
+  <si>
+    <t>2018-05-01 10.jpg</t>
+  </si>
+  <si>
+    <t>Die neuen ESCs sind Bestellt und garantiert bis Freitag angekommen und einsatzbereit</t>
   </si>
 </sst>
 </file>
@@ -909,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C98"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C98" sqref="C98"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2001,6 +2019,39 @@
         <v>188</v>
       </c>
     </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>43221</v>
+      </c>
+      <c r="B99" t="s">
+        <v>190</v>
+      </c>
+      <c r="C99" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>43221</v>
+      </c>
+      <c r="B100" t="s">
+        <v>191</v>
+      </c>
+      <c r="C100" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>43221</v>
+      </c>
+      <c r="B101" t="s">
+        <v>193</v>
+      </c>
+      <c r="C101" t="s">
+        <v>194</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Erster Flug, Notaus und Stop Buttons
</commit_message>
<xml_diff>
--- a/Dokumentation/Schritte.xlsx
+++ b/Dokumentation/Schritte.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="213">
   <si>
     <t>Datum</t>
   </si>
@@ -609,6 +609,60 @@
   </si>
   <si>
     <t>Die neuen ESCs sind Bestellt und garantiert bis Freitag angekommen und einsatzbereit</t>
+  </si>
+  <si>
+    <t>2018-05-04 1.JPG</t>
+  </si>
+  <si>
+    <t>Die ESCs sind angekommen. Der Neue ist etwas größer, kam aber schneller und ist auch für eventuelle stärkere Motoren geeignet</t>
+  </si>
+  <si>
+    <t>2018-05-04 2.JPG</t>
+  </si>
+  <si>
+    <t>Die Teststation ist aufgebaut. Die ersten Flugversuche können gestartet werden</t>
+  </si>
+  <si>
+    <t>2018-05-04 3.JPG</t>
+  </si>
+  <si>
+    <t>Die Teststation von Oben</t>
+  </si>
+  <si>
+    <t>2018-05-04 4.AVI</t>
+  </si>
+  <si>
+    <t>Das erste mal drehen sich die Motoren mit en neuen Platinen, ESCs und Programmen. Auf Anhieb wohl gemerkt !!</t>
+  </si>
+  <si>
+    <t>2018-05-04 5.AVI</t>
+  </si>
+  <si>
+    <t>Der erste Flug aus Sicht der Steuerung. Ausgabe der Drohne, des Arduinos und das GUI</t>
+  </si>
+  <si>
+    <t>2018-05-04 6.AVI</t>
+  </si>
+  <si>
+    <t>Zögerliches Anheben der Rotoren</t>
+  </si>
+  <si>
+    <t>CRASH! Etliche Fehlversuche später und lösen einiger Verbindungsprobleme resultierte dan in diesem Test. Erwartungsgemäß verhielt sich die nicht-kalibirerte Drohne seltsam und zerstörte sich selbst. Wenigstens sind die Motoren jetzt sicher stark genug</t>
+  </si>
+  <si>
+    <t>2018-05-04 7.AVI</t>
+  </si>
+  <si>
+    <t>2018-05-04 8.mp4</t>
+  </si>
+  <si>
+    <t>Der Crash aus sicht des Basiscomputers mit anfänglichen Startschwierigkeiten und meinen Erklärenden Selbstgesprächen (was es sein soll, weiß ich selbst nicht)</t>
+  </si>
+  <si>
+    <t>2018-05-04 9.avi</t>
+  </si>
+  <si>
+    <t>Wir sind jetzt auf YouTube. Der erste Clip wurde zur Demonstration zusammengeschnitten und hochgeladen.</t>
   </si>
 </sst>
 </file>
@@ -927,10 +981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C101" sqref="C101"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2052,6 +2106,105 @@
         <v>194</v>
       </c>
     </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>43224</v>
+      </c>
+      <c r="B102" t="s">
+        <v>195</v>
+      </c>
+      <c r="C102" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>43224</v>
+      </c>
+      <c r="B103" t="s">
+        <v>197</v>
+      </c>
+      <c r="C103" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>43224</v>
+      </c>
+      <c r="B104" t="s">
+        <v>199</v>
+      </c>
+      <c r="C104" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>43224</v>
+      </c>
+      <c r="B105" t="s">
+        <v>201</v>
+      </c>
+      <c r="C105" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>43224</v>
+      </c>
+      <c r="B106" t="s">
+        <v>203</v>
+      </c>
+      <c r="C106" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>43224</v>
+      </c>
+      <c r="B107" t="s">
+        <v>205</v>
+      </c>
+      <c r="C107" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>43224</v>
+      </c>
+      <c r="B108" t="s">
+        <v>208</v>
+      </c>
+      <c r="C108" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>43224</v>
+      </c>
+      <c r="B109" t="s">
+        <v>209</v>
+      </c>
+      <c r="C109" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>43224</v>
+      </c>
+      <c r="B110" t="s">
+        <v>211</v>
+      </c>
+      <c r="C110" t="s">
+        <v>212</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Sensoren auslesen, Zeitaufwand minimiert
</commit_message>
<xml_diff>
--- a/Dokumentation/Schritte.xlsx
+++ b/Dokumentation/Schritte.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Tim\Documents\GitHub\Drohne\Dokumentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\Documents\GitHub\Drohne\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="219">
   <si>
     <t>Datum</t>
   </si>
@@ -669,6 +669,18 @@
   </si>
   <si>
     <t>Das Programm braucht zu lange für berechnungen. Optimierungen werden benötigt!</t>
+  </si>
+  <si>
+    <t>2018-05-06 1.jpg</t>
+  </si>
+  <si>
+    <t>Die Optimierungen sind vorerst abgeschlossen. Eine Berechnungsdauer von ca. 6ms Konnte erzielt werden. Zwar keiner Erstrebten 4ms abeer immerhin besser als 125ms</t>
+  </si>
+  <si>
+    <t>2018-05-06 2.pdf</t>
+  </si>
+  <si>
+    <t>Die Optimierungen bedurften auch einigen Umstrukturierungen auf der Platine. Weshalb die 5. Revision der Kontrollschaltung gemalt wurde</t>
   </si>
 </sst>
 </file>
@@ -987,21 +999,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C111"/>
+  <dimension ref="A1:C113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+      <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="156.42578125" customWidth="1"/>
-    <col min="4" max="1025" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="156.44140625" customWidth="1"/>
+    <col min="4" max="1025" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1012,7 +1024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43032</v>
       </c>
@@ -1023,7 +1035,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43036</v>
       </c>
@@ -1034,7 +1046,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>43042</v>
       </c>
@@ -1045,7 +1057,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>43048</v>
       </c>
@@ -1056,7 +1068,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>43051</v>
       </c>
@@ -1067,7 +1079,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>43058</v>
       </c>
@@ -1078,7 +1090,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>43058</v>
       </c>
@@ -1089,7 +1101,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>43063</v>
       </c>
@@ -1100,7 +1112,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>43063</v>
       </c>
@@ -1111,7 +1123,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>43063</v>
       </c>
@@ -1122,7 +1134,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>43071</v>
       </c>
@@ -1133,7 +1145,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>43071</v>
       </c>
@@ -1144,7 +1156,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>43071</v>
       </c>
@@ -1155,7 +1167,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>43077</v>
       </c>
@@ -1166,7 +1178,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>43078</v>
       </c>
@@ -1177,7 +1189,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>43079</v>
       </c>
@@ -1188,7 +1200,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>43080</v>
       </c>
@@ -1199,7 +1211,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>43090</v>
       </c>
@@ -1210,7 +1222,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>43090</v>
       </c>
@@ -1221,7 +1233,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>43090</v>
       </c>
@@ -1232,7 +1244,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>43091</v>
       </c>
@@ -1243,7 +1255,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>43091</v>
       </c>
@@ -1254,7 +1266,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>43097</v>
       </c>
@@ -1265,7 +1277,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>43097</v>
       </c>
@@ -1276,7 +1288,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>43097</v>
       </c>
@@ -1287,7 +1299,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>43102</v>
       </c>
@@ -1298,7 +1310,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>43101</v>
       </c>
@@ -1309,7 +1321,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>43103</v>
       </c>
@@ -1320,7 +1332,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>43103</v>
       </c>
@@ -1331,7 +1343,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>43103</v>
       </c>
@@ -1342,7 +1354,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>43103</v>
       </c>
@@ -1353,7 +1365,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>43103</v>
       </c>
@@ -1364,7 +1376,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>43103</v>
       </c>
@@ -1375,7 +1387,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>43103</v>
       </c>
@@ -1386,7 +1398,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>43104</v>
       </c>
@@ -1397,7 +1409,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>43105</v>
       </c>
@@ -1408,7 +1420,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>43107</v>
       </c>
@@ -1419,7 +1431,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>43107</v>
       </c>
@@ -1430,7 +1442,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>43111</v>
       </c>
@@ -1441,7 +1453,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>43115</v>
       </c>
@@ -1452,7 +1464,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>43116</v>
       </c>
@@ -1463,7 +1475,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>43114</v>
       </c>
@@ -1474,7 +1486,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43118</v>
       </c>
@@ -1485,7 +1497,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>43118</v>
       </c>
@@ -1496,7 +1508,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>43162</v>
       </c>
@@ -1507,7 +1519,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>43164</v>
       </c>
@@ -1518,7 +1530,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>94</v>
       </c>
@@ -1529,7 +1541,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>43177</v>
       </c>
@@ -1540,7 +1552,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>43183</v>
       </c>
@@ -1551,7 +1563,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>43183</v>
       </c>
@@ -1562,7 +1574,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>43183</v>
       </c>
@@ -1573,7 +1585,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>43187</v>
       </c>
@@ -1584,7 +1596,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>43187</v>
       </c>
@@ -1595,7 +1607,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>43187</v>
       </c>
@@ -1606,7 +1618,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>43187</v>
       </c>
@@ -1617,7 +1629,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>43187</v>
       </c>
@@ -1628,7 +1640,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>43187</v>
       </c>
@@ -1639,7 +1651,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>43187</v>
       </c>
@@ -1650,7 +1662,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>43187</v>
       </c>
@@ -1661,7 +1673,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>43187</v>
       </c>
@@ -1672,7 +1684,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>43188</v>
       </c>
@@ -1683,7 +1695,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>43188</v>
       </c>
@@ -1694,7 +1706,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>43188</v>
       </c>
@@ -1705,7 +1717,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>43188</v>
       </c>
@@ -1716,7 +1728,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>43188</v>
       </c>
@@ -1727,7 +1739,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>43193</v>
       </c>
@@ -1738,7 +1750,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>43194</v>
       </c>
@@ -1749,7 +1761,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>43194</v>
       </c>
@@ -1760,7 +1772,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>43195</v>
       </c>
@@ -1771,7 +1783,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>43195</v>
       </c>
@@ -1782,7 +1794,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>43196</v>
       </c>
@@ -1793,7 +1805,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>43197</v>
       </c>
@@ -1804,7 +1816,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>43199</v>
       </c>
@@ -1815,7 +1827,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>43203</v>
       </c>
@@ -1826,7 +1838,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>43211</v>
       </c>
@@ -1837,7 +1849,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>43211</v>
       </c>
@@ -1848,7 +1860,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>43211</v>
       </c>
@@ -1859,7 +1871,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>43211</v>
       </c>
@@ -1870,7 +1882,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>43211</v>
       </c>
@@ -1881,7 +1893,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>43211</v>
       </c>
@@ -1892,7 +1904,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>43212</v>
       </c>
@@ -1903,7 +1915,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>43212</v>
       </c>
@@ -1914,7 +1926,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>43212</v>
       </c>
@@ -1925,7 +1937,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>43165</v>
       </c>
@@ -1936,7 +1948,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>43215</v>
       </c>
@@ -1947,7 +1959,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>43218</v>
       </c>
@@ -1958,7 +1970,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>43219</v>
       </c>
@@ -1969,7 +1981,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>43219</v>
       </c>
@@ -1980,7 +1992,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>43220</v>
       </c>
@@ -1991,7 +2003,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>43220</v>
       </c>
@@ -2002,7 +2014,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>43221</v>
       </c>
@@ -2013,7 +2025,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>43221</v>
       </c>
@@ -2024,7 +2036,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>43221</v>
       </c>
@@ -2035,7 +2047,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>43221</v>
       </c>
@@ -2046,7 +2058,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>43221</v>
       </c>
@@ -2057,7 +2069,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>43221</v>
       </c>
@@ -2068,7 +2080,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>43221</v>
       </c>
@@ -2079,7 +2091,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>43221</v>
       </c>
@@ -2090,7 +2102,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>43221</v>
       </c>
@@ -2101,7 +2113,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>43221</v>
       </c>
@@ -2112,7 +2124,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>43224</v>
       </c>
@@ -2123,7 +2135,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>43224</v>
       </c>
@@ -2134,7 +2146,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>43224</v>
       </c>
@@ -2145,7 +2157,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>43224</v>
       </c>
@@ -2156,7 +2168,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>43224</v>
       </c>
@@ -2167,7 +2179,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>43224</v>
       </c>
@@ -2178,7 +2190,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>43224</v>
       </c>
@@ -2189,7 +2201,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>43224</v>
       </c>
@@ -2200,7 +2212,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>43224</v>
       </c>
@@ -2211,7 +2223,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>43225</v>
       </c>
@@ -2220,6 +2232,28 @@
       </c>
       <c r="C111" t="s">
         <v>214</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" s="1">
+        <v>43226</v>
+      </c>
+      <c r="B112" t="s">
+        <v>215</v>
+      </c>
+      <c r="C112" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" s="1">
+        <v>43226</v>
+      </c>
+      <c r="B113" t="s">
+        <v>217</v>
+      </c>
+      <c r="C113" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Kommunikation STM Raspberry PI
</commit_message>
<xml_diff>
--- a/Dokumentation/Schritte.xlsx
+++ b/Dokumentation/Schritte.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\Documents\GitHub\Drohne\Dokumentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Tim\Documents\GitHub\Drohne\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="426">
   <si>
     <t>Datum</t>
   </si>
@@ -1291,6 +1291,12 @@
   </si>
   <si>
     <t>Close Up 2</t>
+  </si>
+  <si>
+    <t>2018-08-27.jpg</t>
+  </si>
+  <si>
+    <t>STM und Arduino reden jetzt miteinander. Eine Rekordverdächtige geschwindigkeit von 80us für 10 bytes wurde erreicht. Der Raspberry PI kommt nicht hinterher, hat aber auch Zeit :D</t>
   </si>
 </sst>
 </file>
@@ -1610,21 +1616,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C220"/>
+  <dimension ref="A1:C221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A208" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B221" sqref="B221"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
-    <col min="3" max="3" width="156.44140625" customWidth="1"/>
-    <col min="4" max="1025" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="156.42578125" customWidth="1"/>
+    <col min="4" max="1025" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1635,7 +1641,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43032</v>
       </c>
@@ -1646,7 +1652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43036</v>
       </c>
@@ -1657,7 +1663,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43042</v>
       </c>
@@ -1668,7 +1674,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43048</v>
       </c>
@@ -1679,7 +1685,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43051</v>
       </c>
@@ -1690,7 +1696,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43058</v>
       </c>
@@ -1701,7 +1707,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43058</v>
       </c>
@@ -1712,7 +1718,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43063</v>
       </c>
@@ -1723,7 +1729,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43063</v>
       </c>
@@ -1734,7 +1740,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43063</v>
       </c>
@@ -1745,7 +1751,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43071</v>
       </c>
@@ -1756,7 +1762,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43071</v>
       </c>
@@ -1767,7 +1773,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43071</v>
       </c>
@@ -1778,7 +1784,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43077</v>
       </c>
@@ -1789,7 +1795,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43078</v>
       </c>
@@ -1800,7 +1806,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43079</v>
       </c>
@@ -1811,7 +1817,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43080</v>
       </c>
@@ -1822,7 +1828,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43090</v>
       </c>
@@ -1833,7 +1839,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43090</v>
       </c>
@@ -1844,7 +1850,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43090</v>
       </c>
@@ -1855,7 +1861,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43091</v>
       </c>
@@ -1866,7 +1872,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43091</v>
       </c>
@@ -1877,7 +1883,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43097</v>
       </c>
@@ -1888,7 +1894,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43097</v>
       </c>
@@ -1899,7 +1905,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43097</v>
       </c>
@@ -1910,7 +1916,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43102</v>
       </c>
@@ -1921,7 +1927,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43101</v>
       </c>
@@ -1932,7 +1938,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43103</v>
       </c>
@@ -1943,7 +1949,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43103</v>
       </c>
@@ -1954,7 +1960,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43103</v>
       </c>
@@ -1965,7 +1971,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43103</v>
       </c>
@@ -1976,7 +1982,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43103</v>
       </c>
@@ -1987,7 +1993,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43103</v>
       </c>
@@ -1998,7 +2004,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43103</v>
       </c>
@@ -2009,7 +2015,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43104</v>
       </c>
@@ -2020,7 +2026,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43105</v>
       </c>
@@ -2031,7 +2037,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43107</v>
       </c>
@@ -2042,7 +2048,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43107</v>
       </c>
@@ -2053,7 +2059,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>43111</v>
       </c>
@@ -2064,7 +2070,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43115</v>
       </c>
@@ -2075,7 +2081,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43116</v>
       </c>
@@ -2086,7 +2092,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43114</v>
       </c>
@@ -2097,7 +2103,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43118</v>
       </c>
@@ -2108,7 +2114,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43118</v>
       </c>
@@ -2119,7 +2125,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>43162</v>
       </c>
@@ -2130,7 +2136,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>43164</v>
       </c>
@@ -2141,7 +2147,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>94</v>
       </c>
@@ -2152,7 +2158,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>43177</v>
       </c>
@@ -2163,7 +2169,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>43183</v>
       </c>
@@ -2174,7 +2180,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>43183</v>
       </c>
@@ -2185,7 +2191,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>43183</v>
       </c>
@@ -2196,7 +2202,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>43187</v>
       </c>
@@ -2207,7 +2213,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>43187</v>
       </c>
@@ -2218,7 +2224,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>43187</v>
       </c>
@@ -2229,7 +2235,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>43187</v>
       </c>
@@ -2240,7 +2246,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>43187</v>
       </c>
@@ -2251,7 +2257,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>43187</v>
       </c>
@@ -2262,7 +2268,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>43187</v>
       </c>
@@ -2273,7 +2279,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>43187</v>
       </c>
@@ -2284,7 +2290,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>43187</v>
       </c>
@@ -2295,7 +2301,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>43188</v>
       </c>
@@ -2306,7 +2312,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>43188</v>
       </c>
@@ -2317,7 +2323,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>43188</v>
       </c>
@@ -2328,7 +2334,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>43188</v>
       </c>
@@ -2339,7 +2345,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>43188</v>
       </c>
@@ -2350,7 +2356,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>43193</v>
       </c>
@@ -2361,7 +2367,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>43194</v>
       </c>
@@ -2372,7 +2378,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>43194</v>
       </c>
@@ -2383,7 +2389,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>43195</v>
       </c>
@@ -2394,7 +2400,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>43195</v>
       </c>
@@ -2405,7 +2411,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>43196</v>
       </c>
@@ -2416,7 +2422,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>43197</v>
       </c>
@@ -2427,7 +2433,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>43199</v>
       </c>
@@ -2438,7 +2444,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>43203</v>
       </c>
@@ -2449,7 +2455,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>43211</v>
       </c>
@@ -2460,7 +2466,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>43211</v>
       </c>
@@ -2471,7 +2477,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>43211</v>
       </c>
@@ -2482,7 +2488,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>43211</v>
       </c>
@@ -2493,7 +2499,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>43211</v>
       </c>
@@ -2504,7 +2510,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>43211</v>
       </c>
@@ -2515,7 +2521,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>43212</v>
       </c>
@@ -2526,7 +2532,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>43212</v>
       </c>
@@ -2537,7 +2543,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>43212</v>
       </c>
@@ -2548,7 +2554,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>43165</v>
       </c>
@@ -2559,7 +2565,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>43215</v>
       </c>
@@ -2570,7 +2576,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>43218</v>
       </c>
@@ -2581,7 +2587,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>43219</v>
       </c>
@@ -2592,7 +2598,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>43219</v>
       </c>
@@ -2603,7 +2609,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>43220</v>
       </c>
@@ -2614,7 +2620,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>43220</v>
       </c>
@@ -2625,7 +2631,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>43221</v>
       </c>
@@ -2636,7 +2642,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>43221</v>
       </c>
@@ -2647,7 +2653,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>43221</v>
       </c>
@@ -2658,7 +2664,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>43221</v>
       </c>
@@ -2669,7 +2675,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>43221</v>
       </c>
@@ -2680,7 +2686,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>43221</v>
       </c>
@@ -2691,7 +2697,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>43221</v>
       </c>
@@ -2702,7 +2708,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>43221</v>
       </c>
@@ -2713,7 +2719,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>43221</v>
       </c>
@@ -2724,7 +2730,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>43221</v>
       </c>
@@ -2735,7 +2741,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>43224</v>
       </c>
@@ -2746,7 +2752,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>43224</v>
       </c>
@@ -2757,7 +2763,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>43224</v>
       </c>
@@ -2768,7 +2774,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>43224</v>
       </c>
@@ -2779,7 +2785,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>43224</v>
       </c>
@@ -2790,7 +2796,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>43224</v>
       </c>
@@ -2801,7 +2807,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>43224</v>
       </c>
@@ -2812,7 +2818,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>43224</v>
       </c>
@@ -2823,7 +2829,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>43224</v>
       </c>
@@ -2834,7 +2840,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>43225</v>
       </c>
@@ -2845,7 +2851,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>43226</v>
       </c>
@@ -2856,7 +2862,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>43226</v>
       </c>
@@ -2867,7 +2873,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>43227</v>
       </c>
@@ -2878,7 +2884,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>43228</v>
       </c>
@@ -2889,7 +2895,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>43228</v>
       </c>
@@ -2900,7 +2906,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>43228</v>
       </c>
@@ -2911,7 +2917,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>43228</v>
       </c>
@@ -2922,7 +2928,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>43228</v>
       </c>
@@ -2933,7 +2939,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>43238</v>
       </c>
@@ -2944,7 +2950,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>43246</v>
       </c>
@@ -2955,7 +2961,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>43246</v>
       </c>
@@ -2966,7 +2972,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>43246</v>
       </c>
@@ -2977,7 +2983,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>43246</v>
       </c>
@@ -2988,7 +2994,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>43246</v>
       </c>
@@ -2999,7 +3005,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>43246</v>
       </c>
@@ -3010,7 +3016,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>43246</v>
       </c>
@@ -3021,7 +3027,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>43246</v>
       </c>
@@ -3032,7 +3038,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>43248</v>
       </c>
@@ -3043,7 +3049,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>43248</v>
       </c>
@@ -3054,7 +3060,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>43248</v>
       </c>
@@ -3065,7 +3071,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>43248</v>
       </c>
@@ -3076,7 +3082,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>43248</v>
       </c>
@@ -3087,7 +3093,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>43248</v>
       </c>
@@ -3098,7 +3104,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>43249</v>
       </c>
@@ -3109,7 +3115,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>43249</v>
       </c>
@@ -3120,7 +3126,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>43250</v>
       </c>
@@ -3131,7 +3137,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>43255</v>
       </c>
@@ -3142,7 +3148,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>43258</v>
       </c>
@@ -3153,7 +3159,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>43258</v>
       </c>
@@ -3164,7 +3170,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>43264</v>
       </c>
@@ -3175,7 +3181,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>43264</v>
       </c>
@@ -3186,7 +3192,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>43264</v>
       </c>
@@ -3197,7 +3203,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>43264</v>
       </c>
@@ -3208,7 +3214,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>43265</v>
       </c>
@@ -3219,7 +3225,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>43265</v>
       </c>
@@ -3230,7 +3236,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>43265</v>
       </c>
@@ -3241,7 +3247,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>43265</v>
       </c>
@@ -3252,7 +3258,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>43267</v>
       </c>
@@ -3263,7 +3269,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>43267</v>
       </c>
@@ -3274,7 +3280,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>43267</v>
       </c>
@@ -3285,7 +3291,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>43267</v>
       </c>
@@ -3296,7 +3302,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>43267</v>
       </c>
@@ -3307,7 +3313,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>43267</v>
       </c>
@@ -3318,7 +3324,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>43267</v>
       </c>
@@ -3329,7 +3335,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>43267</v>
       </c>
@@ -3340,7 +3346,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>43267</v>
       </c>
@@ -3351,7 +3357,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>43267</v>
       </c>
@@ -3362,7 +3368,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>43267</v>
       </c>
@@ -3373,7 +3379,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>43267</v>
       </c>
@@ -3384,7 +3390,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>43270</v>
       </c>
@@ -3395,7 +3401,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>43272</v>
       </c>
@@ -3406,7 +3412,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>43273</v>
       </c>
@@ -3417,7 +3423,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>43274</v>
       </c>
@@ -3428,7 +3434,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>43282</v>
       </c>
@@ -3439,7 +3445,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>43294</v>
       </c>
@@ -3450,7 +3456,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>43295</v>
       </c>
@@ -3461,7 +3467,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>43296</v>
       </c>
@@ -3472,7 +3478,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>43296</v>
       </c>
@@ -3483,7 +3489,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>43296</v>
       </c>
@@ -3494,7 +3500,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>43296</v>
       </c>
@@ -3505,7 +3511,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>43297</v>
       </c>
@@ -3516,7 +3522,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>43297</v>
       </c>
@@ -3527,7 +3533,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>43298</v>
       </c>
@@ -3538,7 +3544,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>43298</v>
       </c>
@@ -3549,7 +3555,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>43298</v>
       </c>
@@ -3560,7 +3566,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>43299</v>
       </c>
@@ -3571,7 +3577,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>43300</v>
       </c>
@@ -3582,7 +3588,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>43300</v>
       </c>
@@ -3593,7 +3599,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>43300</v>
       </c>
@@ -3604,7 +3610,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>43300</v>
       </c>
@@ -3615,7 +3621,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>43300</v>
       </c>
@@ -3626,7 +3632,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>43300</v>
       </c>
@@ -3637,7 +3643,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>43300</v>
       </c>
@@ -3648,7 +3654,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>43300</v>
       </c>
@@ -3659,7 +3665,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>43300</v>
       </c>
@@ -3670,7 +3676,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>43302</v>
       </c>
@@ -3681,7 +3687,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>43302</v>
       </c>
@@ -3692,7 +3698,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>43302</v>
       </c>
@@ -3703,7 +3709,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>43302</v>
       </c>
@@ -3714,7 +3720,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>43302</v>
       </c>
@@ -3725,7 +3731,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>43304</v>
       </c>
@@ -3736,7 +3742,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>43304</v>
       </c>
@@ -3747,7 +3753,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>43304</v>
       </c>
@@ -3758,7 +3764,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>43304</v>
       </c>
@@ -3769,7 +3775,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>43304</v>
       </c>
@@ -3780,7 +3786,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>43304</v>
       </c>
@@ -3791,7 +3797,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>43304</v>
       </c>
@@ -3802,7 +3808,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>43304</v>
       </c>
@@ -3813,7 +3819,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>43304</v>
       </c>
@@ -3824,7 +3830,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>43304</v>
       </c>
@@ -3835,7 +3841,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>43304</v>
       </c>
@@ -3846,7 +3852,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>43305</v>
       </c>
@@ -3857,7 +3863,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>43305</v>
       </c>
@@ -3868,7 +3874,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>43314</v>
       </c>
@@ -3879,7 +3885,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>43315</v>
       </c>
@@ -3887,7 +3893,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>43317</v>
       </c>
@@ -3898,7 +3904,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>43317</v>
       </c>
@@ -3909,7 +3915,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>43317</v>
       </c>
@@ -3920,7 +3926,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>43317</v>
       </c>
@@ -3931,7 +3937,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>43317</v>
       </c>
@@ -3942,7 +3948,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>43317</v>
       </c>
@@ -3953,7 +3959,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>43325</v>
       </c>
@@ -3964,7 +3970,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>43325</v>
       </c>
@@ -3975,7 +3981,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>43325</v>
       </c>
@@ -3986,7 +3992,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>43325</v>
       </c>
@@ -3997,7 +4003,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>43325</v>
       </c>
@@ -4008,7 +4014,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>43325</v>
       </c>
@@ -4019,7 +4025,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>43325</v>
       </c>
@@ -4030,7 +4036,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>43325</v>
       </c>
@@ -4039,6 +4045,17 @@
       </c>
       <c r="C220" t="s">
         <v>423</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" s="1">
+        <v>43339</v>
+      </c>
+      <c r="B221" t="s">
+        <v>424</v>
+      </c>
+      <c r="C221" t="s">
+        <v>425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 02. - 05. 9.
</commit_message>
<xml_diff>
--- a/Dokumentation/Schritte.xlsx
+++ b/Dokumentation/Schritte.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\Documents\GitHub\Drohne\Dokumentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Tim\Documents\GitHub\Drohne\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="505">
   <si>
     <t>Datum</t>
   </si>
@@ -1405,6 +1405,135 @@
   </si>
   <si>
     <t>Der Busch war wohl noch nass… Jetzt erstmal trocken werden</t>
+  </si>
+  <si>
+    <t>2018-09-04 1.JPG</t>
+  </si>
+  <si>
+    <t>Nach einem Flugversuch war der kontroller vollkommen entstellt. Nach dem Erfolg ist die konstruktion zu instabil. Da muss was neues her</t>
+  </si>
+  <si>
+    <t>2018-09-02 6.JPG</t>
+  </si>
+  <si>
+    <t>Zunächst muss die powerbank weg. Jetzt wurde eine andere aufgebrochen und die Batterie unter der Drohne befestigt</t>
+  </si>
+  <si>
+    <t>2018-09-02 7.JPG</t>
+  </si>
+  <si>
+    <t>Das Kontroll-Brett mit Ladebuchse, Stromversorgung, Schalter und Ladungsstatus kommt als neues BMS an die alte stelle</t>
+  </si>
+  <si>
+    <t>2018-09-02 8.JPG</t>
+  </si>
+  <si>
+    <t>Hier der Anblick von hinten. Die drohne ist jetzt viel flacher, und die Sensoren sitzen näher am Masse/ Steuerzentrum. Zum an und ausschalten gibt es noch einen Kippschalter</t>
+  </si>
+  <si>
+    <t>2018-09-02 9.JPG</t>
+  </si>
+  <si>
+    <t>Von vorne… Die Drohne ist schon flacher, aber die Schaltbretter müssen noch gerade befestigt werden</t>
+  </si>
+  <si>
+    <t>2018-09-02 10.JPG</t>
+  </si>
+  <si>
+    <t>Die lösung auf das problem mit den vielen Steckern vom Rahmen zum Controller wurde jetzt in die Hand genommen und zusammengefasst</t>
+  </si>
+  <si>
+    <t>Die Batterie hat jetzt auch ein sicheres Abteil und die Kamera einen Platz…</t>
+  </si>
+  <si>
+    <t>2018-09-04 2.JPG</t>
+  </si>
+  <si>
+    <t>Das Gesicht der neuen Drohne</t>
+  </si>
+  <si>
+    <t>2018-09-04 3.JPG</t>
+  </si>
+  <si>
+    <t>Die Sicht der Drohne</t>
+  </si>
+  <si>
+    <t>2018-09-04 4.JPG</t>
+  </si>
+  <si>
+    <t>Trotz feuchtem Wetter muss mit dem neuen aufbau ein neuer Testflug geflogen werden</t>
+  </si>
+  <si>
+    <t>2018-09-04 6.JPG</t>
+  </si>
+  <si>
+    <t>Patrick ist da, um schöne Bilder zu machen. Diesmal wird es sogar Hochaufgelöst</t>
+  </si>
+  <si>
+    <t>2018-09-04 5.JPG</t>
+  </si>
+  <si>
+    <t>Aufschalten auf die Drohne</t>
+  </si>
+  <si>
+    <t>2018-09-04 7.MOV</t>
+  </si>
+  <si>
+    <t>Die Drohne hebt nicht ab. Es waren 2 Propeller falsch rum draufgesessen</t>
+  </si>
+  <si>
+    <t>2018-09-04 8.MOV</t>
+  </si>
+  <si>
+    <t>Schon  wieder ein absturz. Das ist niederschmetternd. Nach dem erfolg vor 2 Tagen, dachte ich, wir könnten es schaffen. Jetzt bin ich Zeitmäßig wieder 2-3 Tage los.</t>
+  </si>
+  <si>
+    <t>Heute ist schönes Wetter. Zeit um dem Problemen von Gestern nachzugehen. Der Start ist gut, bloß dann wieder, ein Salto</t>
+  </si>
+  <si>
+    <t>Und wieder</t>
+  </si>
+  <si>
+    <t>2018-09-05 3.mp4</t>
+  </si>
+  <si>
+    <t>2018-09-05 2.AVI</t>
+  </si>
+  <si>
+    <t>2018-09-05 1.AVI</t>
+  </si>
+  <si>
+    <t>2018-09-05 4.mp4</t>
+  </si>
+  <si>
+    <t>Falsche Propeller</t>
+  </si>
+  <si>
+    <t>2018-09-05 5.mp4</t>
+  </si>
+  <si>
+    <t>2018-09-05 6.AVI</t>
+  </si>
+  <si>
+    <t>Dieser Flug war schon wieder Okay. So gut, wie man mit einer Zeitverzögerung von 1-2s halt fliegen kann. Fernsteuern ist langsam aussichtslos</t>
+  </si>
+  <si>
+    <t>2018-09-05 7.AVI</t>
+  </si>
+  <si>
+    <t>Die Flüge werden immer besser. Ich kann die richtung einigermaßen bestimmen und die Drohne steht gerade in der Luft. Nur das reagieren auf das steigen und sinken der Drohne funktioniert nicht</t>
+  </si>
+  <si>
+    <t>2018-09-05 8.mp4</t>
+  </si>
+  <si>
+    <t>Apropos steigen und sinken. Den Kirschbaum brauchen wir auch nicht mehr schneiden :)</t>
+  </si>
+  <si>
+    <t>2018-09-05 9.mp4</t>
+  </si>
+  <si>
+    <t>Kontrollieren der richtungen in trocken+bungen. Soweit scheint alles zu klappen. Wüde die Drohne nicht abdriften, könnte man schon die erste automatation reinbringen</t>
   </si>
 </sst>
 </file>
@@ -1724,21 +1853,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C239"/>
+  <dimension ref="A1:C262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A211" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C239" sqref="C239"/>
+    <sheetView tabSelected="1" topLeftCell="A232" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B263" sqref="B263"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
-    <col min="3" max="3" width="156.44140625" customWidth="1"/>
-    <col min="4" max="1025" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="156.42578125" customWidth="1"/>
+    <col min="4" max="1025" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1749,7 +1878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43032</v>
       </c>
@@ -1760,7 +1889,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43036</v>
       </c>
@@ -1771,7 +1900,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43042</v>
       </c>
@@ -1782,7 +1911,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43048</v>
       </c>
@@ -1793,7 +1922,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43051</v>
       </c>
@@ -1804,7 +1933,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43058</v>
       </c>
@@ -1815,7 +1944,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43058</v>
       </c>
@@ -1826,7 +1955,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43063</v>
       </c>
@@ -1837,7 +1966,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43063</v>
       </c>
@@ -1848,7 +1977,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43063</v>
       </c>
@@ -1859,7 +1988,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43071</v>
       </c>
@@ -1870,7 +1999,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43071</v>
       </c>
@@ -1881,7 +2010,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43071</v>
       </c>
@@ -1892,7 +2021,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43077</v>
       </c>
@@ -1903,7 +2032,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43078</v>
       </c>
@@ -1914,7 +2043,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43079</v>
       </c>
@@ -1925,7 +2054,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43080</v>
       </c>
@@ -1936,7 +2065,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43090</v>
       </c>
@@ -1947,7 +2076,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43090</v>
       </c>
@@ -1958,7 +2087,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43090</v>
       </c>
@@ -1969,7 +2098,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43091</v>
       </c>
@@ -1980,7 +2109,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43091</v>
       </c>
@@ -1991,7 +2120,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43097</v>
       </c>
@@ -2002,7 +2131,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43097</v>
       </c>
@@ -2013,7 +2142,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43097</v>
       </c>
@@ -2024,7 +2153,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43102</v>
       </c>
@@ -2035,7 +2164,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43101</v>
       </c>
@@ -2046,7 +2175,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43103</v>
       </c>
@@ -2057,7 +2186,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43103</v>
       </c>
@@ -2068,7 +2197,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43103</v>
       </c>
@@ -2079,7 +2208,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43103</v>
       </c>
@@ -2090,7 +2219,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43103</v>
       </c>
@@ -2101,7 +2230,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43103</v>
       </c>
@@ -2112,7 +2241,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43103</v>
       </c>
@@ -2123,7 +2252,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43104</v>
       </c>
@@ -2134,7 +2263,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43105</v>
       </c>
@@ -2145,7 +2274,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43107</v>
       </c>
@@ -2156,7 +2285,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43107</v>
       </c>
@@ -2167,7 +2296,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>43111</v>
       </c>
@@ -2178,7 +2307,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43115</v>
       </c>
@@ -2189,7 +2318,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43116</v>
       </c>
@@ -2200,7 +2329,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43114</v>
       </c>
@@ -2211,7 +2340,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43118</v>
       </c>
@@ -2222,7 +2351,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43118</v>
       </c>
@@ -2233,7 +2362,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>43162</v>
       </c>
@@ -2244,7 +2373,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>43164</v>
       </c>
@@ -2255,7 +2384,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>94</v>
       </c>
@@ -2266,7 +2395,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>43177</v>
       </c>
@@ -2277,7 +2406,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>43183</v>
       </c>
@@ -2288,7 +2417,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>43183</v>
       </c>
@@ -2299,7 +2428,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>43183</v>
       </c>
@@ -2310,7 +2439,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>43187</v>
       </c>
@@ -2321,7 +2450,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>43187</v>
       </c>
@@ -2332,7 +2461,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>43187</v>
       </c>
@@ -2343,7 +2472,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>43187</v>
       </c>
@@ -2354,7 +2483,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>43187</v>
       </c>
@@ -2365,7 +2494,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>43187</v>
       </c>
@@ -2376,7 +2505,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>43187</v>
       </c>
@@ -2387,7 +2516,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>43187</v>
       </c>
@@ -2398,7 +2527,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>43187</v>
       </c>
@@ -2409,7 +2538,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>43188</v>
       </c>
@@ -2420,7 +2549,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>43188</v>
       </c>
@@ -2431,7 +2560,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>43188</v>
       </c>
@@ -2442,7 +2571,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>43188</v>
       </c>
@@ -2453,7 +2582,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>43188</v>
       </c>
@@ -2464,7 +2593,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>43193</v>
       </c>
@@ -2475,7 +2604,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>43194</v>
       </c>
@@ -2486,7 +2615,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>43194</v>
       </c>
@@ -2497,7 +2626,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>43195</v>
       </c>
@@ -2508,7 +2637,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>43195</v>
       </c>
@@ -2519,7 +2648,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>43196</v>
       </c>
@@ -2530,7 +2659,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>43197</v>
       </c>
@@ -2541,7 +2670,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>43199</v>
       </c>
@@ -2552,7 +2681,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>43203</v>
       </c>
@@ -2563,7 +2692,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>43211</v>
       </c>
@@ -2574,7 +2703,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>43211</v>
       </c>
@@ -2585,7 +2714,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>43211</v>
       </c>
@@ -2596,7 +2725,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>43211</v>
       </c>
@@ -2607,7 +2736,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>43211</v>
       </c>
@@ -2618,7 +2747,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>43211</v>
       </c>
@@ -2629,7 +2758,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>43212</v>
       </c>
@@ -2640,7 +2769,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>43212</v>
       </c>
@@ -2651,7 +2780,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>43212</v>
       </c>
@@ -2662,7 +2791,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>43165</v>
       </c>
@@ -2673,7 +2802,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>43215</v>
       </c>
@@ -2684,7 +2813,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>43218</v>
       </c>
@@ -2695,7 +2824,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>43219</v>
       </c>
@@ -2706,7 +2835,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>43219</v>
       </c>
@@ -2717,7 +2846,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>43220</v>
       </c>
@@ -2728,7 +2857,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>43220</v>
       </c>
@@ -2739,7 +2868,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>43221</v>
       </c>
@@ -2750,7 +2879,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>43221</v>
       </c>
@@ -2761,7 +2890,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>43221</v>
       </c>
@@ -2772,7 +2901,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>43221</v>
       </c>
@@ -2783,7 +2912,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>43221</v>
       </c>
@@ -2794,7 +2923,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>43221</v>
       </c>
@@ -2805,7 +2934,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>43221</v>
       </c>
@@ -2816,7 +2945,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>43221</v>
       </c>
@@ -2827,7 +2956,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>43221</v>
       </c>
@@ -2838,7 +2967,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>43221</v>
       </c>
@@ -2849,7 +2978,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>43224</v>
       </c>
@@ -2860,7 +2989,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>43224</v>
       </c>
@@ -2871,7 +3000,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>43224</v>
       </c>
@@ -2882,7 +3011,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>43224</v>
       </c>
@@ -2893,7 +3022,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>43224</v>
       </c>
@@ -2904,7 +3033,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>43224</v>
       </c>
@@ -2915,7 +3044,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>43224</v>
       </c>
@@ -2926,7 +3055,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>43224</v>
       </c>
@@ -2937,7 +3066,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>43224</v>
       </c>
@@ -2948,7 +3077,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>43225</v>
       </c>
@@ -2959,7 +3088,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>43226</v>
       </c>
@@ -2970,7 +3099,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>43226</v>
       </c>
@@ -2981,7 +3110,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>43227</v>
       </c>
@@ -2992,7 +3121,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>43228</v>
       </c>
@@ -3003,7 +3132,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>43228</v>
       </c>
@@ -3014,7 +3143,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>43228</v>
       </c>
@@ -3025,7 +3154,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>43228</v>
       </c>
@@ -3036,7 +3165,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>43228</v>
       </c>
@@ -3047,7 +3176,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>43238</v>
       </c>
@@ -3058,7 +3187,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>43246</v>
       </c>
@@ -3069,7 +3198,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>43246</v>
       </c>
@@ -3080,7 +3209,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>43246</v>
       </c>
@@ -3091,7 +3220,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>43246</v>
       </c>
@@ -3102,7 +3231,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>43246</v>
       </c>
@@ -3113,7 +3242,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>43246</v>
       </c>
@@ -3124,7 +3253,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>43246</v>
       </c>
@@ -3135,7 +3264,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>43246</v>
       </c>
@@ -3146,7 +3275,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>43248</v>
       </c>
@@ -3157,7 +3286,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>43248</v>
       </c>
@@ -3168,7 +3297,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>43248</v>
       </c>
@@ -3179,7 +3308,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>43248</v>
       </c>
@@ -3190,7 +3319,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>43248</v>
       </c>
@@ -3201,7 +3330,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>43248</v>
       </c>
@@ -3212,7 +3341,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>43249</v>
       </c>
@@ -3223,7 +3352,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>43249</v>
       </c>
@@ -3234,7 +3363,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>43250</v>
       </c>
@@ -3245,7 +3374,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>43255</v>
       </c>
@@ -3256,7 +3385,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>43258</v>
       </c>
@@ -3267,7 +3396,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>43258</v>
       </c>
@@ -3278,7 +3407,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>43264</v>
       </c>
@@ -3289,7 +3418,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>43264</v>
       </c>
@@ -3300,7 +3429,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>43264</v>
       </c>
@@ -3311,7 +3440,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>43264</v>
       </c>
@@ -3322,7 +3451,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>43265</v>
       </c>
@@ -3333,7 +3462,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>43265</v>
       </c>
@@ -3344,7 +3473,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>43265</v>
       </c>
@@ -3355,7 +3484,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>43265</v>
       </c>
@@ -3366,7 +3495,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>43267</v>
       </c>
@@ -3377,7 +3506,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>43267</v>
       </c>
@@ -3388,7 +3517,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>43267</v>
       </c>
@@ -3399,7 +3528,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>43267</v>
       </c>
@@ -3410,7 +3539,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>43267</v>
       </c>
@@ -3421,7 +3550,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>43267</v>
       </c>
@@ -3432,7 +3561,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>43267</v>
       </c>
@@ -3443,7 +3572,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>43267</v>
       </c>
@@ -3454,7 +3583,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>43267</v>
       </c>
@@ -3465,7 +3594,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>43267</v>
       </c>
@@ -3476,7 +3605,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>43267</v>
       </c>
@@ -3487,7 +3616,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>43267</v>
       </c>
@@ -3498,7 +3627,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>43270</v>
       </c>
@@ -3509,7 +3638,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>43272</v>
       </c>
@@ -3520,7 +3649,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>43273</v>
       </c>
@@ -3531,7 +3660,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>43274</v>
       </c>
@@ -3542,7 +3671,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>43282</v>
       </c>
@@ -3553,7 +3682,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>43294</v>
       </c>
@@ -3564,7 +3693,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>43295</v>
       </c>
@@ -3575,7 +3704,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>43296</v>
       </c>
@@ -3586,7 +3715,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>43296</v>
       </c>
@@ -3597,7 +3726,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>43296</v>
       </c>
@@ -3608,7 +3737,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>43296</v>
       </c>
@@ -3619,7 +3748,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>43297</v>
       </c>
@@ -3630,7 +3759,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>43297</v>
       </c>
@@ -3641,7 +3770,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>43298</v>
       </c>
@@ -3652,7 +3781,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>43298</v>
       </c>
@@ -3663,7 +3792,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>43298</v>
       </c>
@@ -3674,7 +3803,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>43299</v>
       </c>
@@ -3685,7 +3814,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>43300</v>
       </c>
@@ -3696,7 +3825,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>43300</v>
       </c>
@@ -3707,7 +3836,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>43300</v>
       </c>
@@ -3718,7 +3847,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>43300</v>
       </c>
@@ -3729,7 +3858,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>43300</v>
       </c>
@@ -3740,7 +3869,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>43300</v>
       </c>
@@ -3751,7 +3880,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>43300</v>
       </c>
@@ -3762,7 +3891,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>43300</v>
       </c>
@@ -3773,7 +3902,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>43300</v>
       </c>
@@ -3784,7 +3913,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>43302</v>
       </c>
@@ -3795,7 +3924,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>43302</v>
       </c>
@@ -3806,7 +3935,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>43302</v>
       </c>
@@ -3817,7 +3946,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>43302</v>
       </c>
@@ -3828,7 +3957,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>43302</v>
       </c>
@@ -3839,7 +3968,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>43304</v>
       </c>
@@ -3850,7 +3979,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>43304</v>
       </c>
@@ -3861,7 +3990,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>43304</v>
       </c>
@@ -3872,7 +4001,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>43304</v>
       </c>
@@ -3883,7 +4012,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>43304</v>
       </c>
@@ -3894,7 +4023,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>43304</v>
       </c>
@@ -3905,7 +4034,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>43304</v>
       </c>
@@ -3916,7 +4045,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>43304</v>
       </c>
@@ -3927,7 +4056,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>43304</v>
       </c>
@@ -3938,7 +4067,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>43304</v>
       </c>
@@ -3949,7 +4078,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>43304</v>
       </c>
@@ -3960,7 +4089,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>43305</v>
       </c>
@@ -3971,7 +4100,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>43305</v>
       </c>
@@ -3982,7 +4111,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>43314</v>
       </c>
@@ -3993,7 +4122,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>43315</v>
       </c>
@@ -4001,7 +4130,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>43317</v>
       </c>
@@ -4012,7 +4141,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>43317</v>
       </c>
@@ -4023,7 +4152,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>43317</v>
       </c>
@@ -4034,7 +4163,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>43317</v>
       </c>
@@ -4045,7 +4174,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>43317</v>
       </c>
@@ -4056,7 +4185,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>43317</v>
       </c>
@@ -4067,7 +4196,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>43325</v>
       </c>
@@ -4078,7 +4207,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>43325</v>
       </c>
@@ -4089,7 +4218,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>43325</v>
       </c>
@@ -4100,7 +4229,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>43325</v>
       </c>
@@ -4111,7 +4240,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>43325</v>
       </c>
@@ -4122,7 +4251,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>43325</v>
       </c>
@@ -4133,7 +4262,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>43325</v>
       </c>
@@ -4144,7 +4273,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>43325</v>
       </c>
@@ -4155,7 +4284,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>43339</v>
       </c>
@@ -4166,7 +4295,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>43339</v>
       </c>
@@ -4177,7 +4306,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>43327</v>
       </c>
@@ -4188,7 +4317,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>43340</v>
       </c>
@@ -4199,7 +4328,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>43340</v>
       </c>
@@ -4210,7 +4339,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>43342</v>
       </c>
@@ -4221,7 +4350,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>43342</v>
       </c>
@@ -4232,7 +4361,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>43340</v>
       </c>
@@ -4243,7 +4372,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>43344</v>
       </c>
@@ -4254,7 +4383,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>43344</v>
       </c>
@@ -4265,7 +4394,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>43344</v>
       </c>
@@ -4276,7 +4405,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>43344</v>
       </c>
@@ -4287,7 +4416,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>43344</v>
       </c>
@@ -4298,7 +4427,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>43344</v>
       </c>
@@ -4309,7 +4438,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>43344</v>
       </c>
@@ -4320,7 +4449,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>43345</v>
       </c>
@@ -4331,7 +4460,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>43345</v>
       </c>
@@ -4342,7 +4471,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>43345</v>
       </c>
@@ -4353,7 +4482,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>43345</v>
       </c>
@@ -4362,6 +4491,259 @@
       </c>
       <c r="C239" t="s">
         <v>461</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A240" s="1">
+        <v>43345</v>
+      </c>
+      <c r="B240" t="s">
+        <v>462</v>
+      </c>
+      <c r="C240" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241" s="1">
+        <v>43345</v>
+      </c>
+      <c r="B241" t="s">
+        <v>464</v>
+      </c>
+      <c r="C241" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" s="1">
+        <v>43345</v>
+      </c>
+      <c r="B242" t="s">
+        <v>466</v>
+      </c>
+      <c r="C242" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" s="1">
+        <v>43345</v>
+      </c>
+      <c r="B243" t="s">
+        <v>468</v>
+      </c>
+      <c r="C243" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244" s="1">
+        <v>43345</v>
+      </c>
+      <c r="B244" t="s">
+        <v>470</v>
+      </c>
+      <c r="C244" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245" s="1">
+        <v>43345</v>
+      </c>
+      <c r="B245" t="s">
+        <v>472</v>
+      </c>
+      <c r="C245" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A246" s="1">
+        <v>43347</v>
+      </c>
+      <c r="B246" t="s">
+        <v>462</v>
+      </c>
+      <c r="C246" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A247" s="1">
+        <v>43347</v>
+      </c>
+      <c r="B247" t="s">
+        <v>475</v>
+      </c>
+      <c r="C247" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A248" s="1">
+        <v>43347</v>
+      </c>
+      <c r="B248" t="s">
+        <v>477</v>
+      </c>
+      <c r="C248" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A249" s="1">
+        <v>43347</v>
+      </c>
+      <c r="B249" t="s">
+        <v>479</v>
+      </c>
+      <c r="C249" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A250" s="1">
+        <v>43347</v>
+      </c>
+      <c r="B250" t="s">
+        <v>483</v>
+      </c>
+      <c r="C250" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A251" s="1">
+        <v>43347</v>
+      </c>
+      <c r="B251" t="s">
+        <v>481</v>
+      </c>
+      <c r="C251" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A252" s="1">
+        <v>43347</v>
+      </c>
+      <c r="B252" t="s">
+        <v>485</v>
+      </c>
+      <c r="C252" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A253" s="1">
+        <v>43347</v>
+      </c>
+      <c r="B253" t="s">
+        <v>487</v>
+      </c>
+      <c r="C253" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A254" s="1">
+        <v>43348</v>
+      </c>
+      <c r="B254" t="s">
+        <v>493</v>
+      </c>
+      <c r="C254" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A255" s="1">
+        <v>43348</v>
+      </c>
+      <c r="B255" t="s">
+        <v>492</v>
+      </c>
+      <c r="C255" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A256" s="1">
+        <v>43348</v>
+      </c>
+      <c r="B256" t="s">
+        <v>491</v>
+      </c>
+      <c r="C256" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A257" s="1">
+        <v>43348</v>
+      </c>
+      <c r="B257" t="s">
+        <v>494</v>
+      </c>
+      <c r="C257" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A258" s="1">
+        <v>43348</v>
+      </c>
+      <c r="B258" t="s">
+        <v>496</v>
+      </c>
+      <c r="C258" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A259" s="1">
+        <v>43348</v>
+      </c>
+      <c r="B259" t="s">
+        <v>497</v>
+      </c>
+      <c r="C259" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A260" s="1">
+        <v>43348</v>
+      </c>
+      <c r="B260" t="s">
+        <v>499</v>
+      </c>
+      <c r="C260" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A261" s="1">
+        <v>43348</v>
+      </c>
+      <c r="B261" t="s">
+        <v>501</v>
+      </c>
+      <c r="C261" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A262" s="1">
+        <v>43348</v>
+      </c>
+      <c r="B262" t="s">
+        <v>503</v>
+      </c>
+      <c r="C262" t="s">
+        <v>504</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
YMFC v2 und Kommunikation verbessert
</commit_message>
<xml_diff>
--- a/Dokumentation/Schritte.xlsx
+++ b/Dokumentation/Schritte.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="549">
   <si>
     <t>Datum</t>
   </si>
@@ -1624,6 +1624,48 @@
   </si>
   <si>
     <t>2018-09-09 5.jpg</t>
+  </si>
+  <si>
+    <t>2018-09-16.jpg</t>
+  </si>
+  <si>
+    <t>Gut, dass wir github benutzen. Es ist ein Unfall beim Hochladen von Dateien passiert</t>
+  </si>
+  <si>
+    <t>2018-09-21 1.JPG</t>
+  </si>
+  <si>
+    <t>Das gehäuse für den höhensensor wurde gedruckt. Jetzt läuft er hoffentlich besser</t>
+  </si>
+  <si>
+    <t>Nahaufnahme</t>
+  </si>
+  <si>
+    <t>2018-09-21 2.JPG</t>
+  </si>
+  <si>
+    <t>Das Oszilloskop ist weg. Jetzt muss ich wieder einen Arduino zum debuggen der Leitungen verwenden</t>
+  </si>
+  <si>
+    <t>2018-09-27 2.AVI</t>
+  </si>
+  <si>
+    <t>Endlich dreht sich der Rotor wieder. Diesmal von einem anderen Anschluss</t>
+  </si>
+  <si>
+    <t>2018-09-27 1.JPG</t>
+  </si>
+  <si>
+    <t>2018-09-27 3.AVI</t>
+  </si>
+  <si>
+    <t>Und alle 4. Das ist immer gar nicht so leicht, wie man sich es vorstellt</t>
+  </si>
+  <si>
+    <t>2018-09-29.pdf</t>
+  </si>
+  <si>
+    <t>Die neusten (auch älteren) änderungen an der kontrollschaltung wurden upgedated. Außerdem muss der neue YMFC umgeschrieben werden, sodass ich nach 8h tippen sagen kann, dass meine finger bluten! :)</t>
   </si>
 </sst>
 </file>
@@ -1943,10 +1985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C278"/>
+  <dimension ref="A1:C285"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A256" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B280" sqref="B280"/>
+      <selection activeCell="C281" sqref="C281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5012,6 +5054,83 @@
         <v>533</v>
       </c>
     </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A279" s="1">
+        <v>43359</v>
+      </c>
+      <c r="B279" t="s">
+        <v>535</v>
+      </c>
+      <c r="C279" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A280" s="1">
+        <v>43364</v>
+      </c>
+      <c r="B280" t="s">
+        <v>537</v>
+      </c>
+      <c r="C280" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A281" s="1">
+        <v>43364</v>
+      </c>
+      <c r="B281" t="s">
+        <v>540</v>
+      </c>
+      <c r="C281" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A282" s="1">
+        <v>43370</v>
+      </c>
+      <c r="B282" t="s">
+        <v>544</v>
+      </c>
+      <c r="C282" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A283" s="1">
+        <v>43370</v>
+      </c>
+      <c r="B283" t="s">
+        <v>542</v>
+      </c>
+      <c r="C283" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A284" s="1">
+        <v>43370</v>
+      </c>
+      <c r="B284" t="s">
+        <v>545</v>
+      </c>
+      <c r="C284" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A285" s="1">
+        <v>43372</v>
+      </c>
+      <c r="B285" t="s">
+        <v>547</v>
+      </c>
+      <c r="C285" t="s">
+        <v>548</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Letzte Dokumentationen (bis 30.10.)
</commit_message>
<xml_diff>
--- a/Dokumentation/Schritte.xlsx
+++ b/Dokumentation/Schritte.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="581">
   <si>
     <t>Datum</t>
   </si>
@@ -1717,6 +1717,51 @@
   </si>
   <si>
     <t>Der Höhensensor auf der Drohne in nahaufnahme (hab ich schon vor ein paar tagen gemacht, aber Dokumentation ist aufwendig)</t>
+  </si>
+  <si>
+    <t>Vorletzter Entwicklungstag</t>
+  </si>
+  <si>
+    <t>Letzter Entwicklungstag</t>
+  </si>
+  <si>
+    <t>2018-10-14 1.JPG</t>
+  </si>
+  <si>
+    <t>2018-10-21 2.JPG</t>
+  </si>
+  <si>
+    <t>Drohne stürzt bei versuch ab, Kabel schmoren durch das Zimmer stikt. Gott sei dank steht das Haus noch</t>
+  </si>
+  <si>
+    <t>2018-10-14 2.JPG</t>
+  </si>
+  <si>
+    <t>2018-10-14 3.JPG</t>
+  </si>
+  <si>
+    <t>2018-10-21 3.JPG</t>
+  </si>
+  <si>
+    <t>Höhensensor ist gekommen zum Ausprobieren</t>
+  </si>
+  <si>
+    <t>Bei einem weiteren Flugversuch macht ein Motor seltsame geräusche. Bis man den winzigen stein gefunden hat vergehen auch wieder ewigkeiten</t>
+  </si>
+  <si>
+    <t>2018-10-21 1.JPG</t>
+  </si>
+  <si>
+    <t>2018-10-30.JPG</t>
+  </si>
+  <si>
+    <t>Wie viel Pech muss man haben, dass der SD-Kartenleser am Raspi kaputt geht??? Nichts, was sich nicht lösen ließe</t>
+  </si>
+  <si>
+    <t>Upgrade auf GPS-Sensor (unten) und umrüstung auf den RasPi3</t>
+  </si>
+  <si>
+    <t>Die Löstspitze ist inzwischen auch durchgerostet und fast zerstört XD</t>
   </si>
 </sst>
 </file>
@@ -2036,10 +2081,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C294"/>
+  <dimension ref="A1:C303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A258" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C294" sqref="C294"/>
+    <sheetView tabSelected="1" topLeftCell="A280" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C301" sqref="C301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5281,6 +5326,99 @@
         <v>278</v>
       </c>
     </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A295" s="1">
+        <v>43387</v>
+      </c>
+      <c r="B295" t="s">
+        <v>568</v>
+      </c>
+      <c r="C295" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A296" s="1">
+        <v>43387</v>
+      </c>
+      <c r="B296" t="s">
+        <v>571</v>
+      </c>
+      <c r="C296" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A297" s="1">
+        <v>43387</v>
+      </c>
+      <c r="B297" t="s">
+        <v>572</v>
+      </c>
+      <c r="C297" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A298" s="1">
+        <v>43394</v>
+      </c>
+      <c r="B298" t="s">
+        <v>576</v>
+      </c>
+      <c r="C298" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A299" s="1">
+        <v>43394</v>
+      </c>
+      <c r="B299" t="s">
+        <v>569</v>
+      </c>
+      <c r="C299" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A300" s="1">
+        <v>43394</v>
+      </c>
+      <c r="B300" t="s">
+        <v>573</v>
+      </c>
+      <c r="C300" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A301" s="1">
+        <v>43403</v>
+      </c>
+      <c r="B301" t="s">
+        <v>577</v>
+      </c>
+      <c r="C301" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A302" s="1">
+        <v>43421</v>
+      </c>
+      <c r="C302" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A303" s="1">
+        <v>43422</v>
+      </c>
+      <c r="C303" t="s">
+        <v>567</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>